<commit_message>
Spotted a mistake with ground in the schematic
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="184">
   <si>
     <t>Key</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Aquired</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Ordered</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>LTC6907CS6#TRMPBF </t>
   </si>
   <si>
-    <t>http://uk.farnell.com/linear-technology/ltc6907cs6-trmpbf/oscillator-40khz-4mhz-tsot23-6/dp/1663929?st=LTC6907CS6#TRMPBF</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
   </si>
   <si>
     <t>T9, T10, T11, T12</t>
-  </si>
-  <si>
-    <t>Dup</t>
   </si>
   <si>
     <t>R5, R6, R7, R8</t>
@@ -599,16 +590,86 @@
   <si>
     <t>http://uk.farnell.com/multicomp/mcwr08x1001ftl/res-thick-film-1k-1-0-125w-0805/dp/2447587</t>
   </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>2 Pos Header MF</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>2 Pos Receptacle MF</t>
+  </si>
+  <si>
+    <t>39-01-2020</t>
+  </si>
+  <si>
+    <t>484-1748</t>
+  </si>
+  <si>
+    <t>Mini-fit Jr Crimp</t>
+  </si>
+  <si>
+    <t>39-00-0038</t>
+  </si>
+  <si>
+    <t>670-6307 </t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/4841748/</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-contacts/6706307/</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/linear-technology/ltc6907cs6-trmpbf/oscillator-40khz-4mhz-tsot23-6/dp/1663929RL</t>
+  </si>
+  <si>
+    <t>484-1883 </t>
+  </si>
+  <si>
+    <t>39-28-1023</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-headers/4841883/</t>
+  </si>
+  <si>
+    <t>3.5 mm Audio Cable</t>
+  </si>
+  <si>
+    <t>Pro Signal</t>
+  </si>
+  <si>
+    <t>AV13646</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/pro-signal/av13646/lead-3-5mm-s-jack-jack-1-2m/dp/3712278</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>2 (Dup)</t>
+  </si>
+  <si>
+    <t>3 (Dup)</t>
+  </si>
+  <si>
+    <t>4 (Dup)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="\£#,##0.000;[Red]&quot;-£&quot;#,##0.000"/>
     <numFmt numFmtId="165" formatCode="\£#,##0.00;[Red]&quot;-£&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\£#,##0.000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.000;[Red]\-[$£-809]#,##0.000"/>
+    <numFmt numFmtId="178" formatCode="0.000000000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -652,7 +713,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,12 +752,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor rgb="FFFF00FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF993300"/>
       </patternFill>
@@ -717,6 +772,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -760,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -786,7 +865,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -797,20 +875,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -820,8 +892,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1281,7 @@
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375"/>
     <col min="10" max="10" width="15.42578125"/>
-    <col min="11" max="11" width="253"/>
+    <col min="11" max="11" width="94.85546875" customWidth="1"/>
     <col min="12" max="26" width="8.5703125"/>
     <col min="27" max="1025" width="14.140625"/>
   </cols>
@@ -1203,26 +1297,24 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="E4" s="47"/>
       <c r="F4" s="6"/>
       <c r="J4" s="1"/>
     </row>
@@ -1231,35 +1323,35 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1267,7 +1359,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8">
@@ -1277,31 +1369,31 @@
         <v>2</v>
       </c>
       <c r="E8" s="10">
-        <f t="shared" ref="E8:E16" si="0">C8*D8</f>
+        <f t="shared" ref="E8:E47" si="0">C8*D8</f>
         <v>2.46E-2</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>134</v>
+      <c r="F8" s="29" t="s">
+        <v>131</v>
       </c>
       <c r="G8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="J8" s="11">
         <v>2074393</v>
       </c>
       <c r="K8" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>22</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8">
@@ -1314,28 +1406,28 @@
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>23</v>
+      <c r="F9" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" s="11">
         <v>2447587</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8">
@@ -1348,28 +1440,28 @@
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>135</v>
+      <c r="F10" s="29" t="s">
+        <v>132</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" s="11">
         <v>2447601</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="12">
@@ -1382,28 +1474,28 @@
         <f t="shared" si="0"/>
         <v>1.7600000000000001E-2</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="I11" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="11">
         <v>1759226</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8">
@@ -1416,28 +1508,28 @@
         <f t="shared" si="0"/>
         <v>0.11399999999999999</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>33</v>
+      <c r="F12" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="11">
         <v>2320821</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="8">
@@ -1450,30 +1542,30 @@
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="B14" s="28"/>
       <c r="C14" s="8">
         <v>0.75600000000000001</v>
       </c>
@@ -1484,30 +1576,30 @@
         <f t="shared" si="0"/>
         <v>0.75600000000000001</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="I14" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="11">
         <v>8044953</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="13"/>
+        <v>43</v>
+      </c>
+      <c r="B15" s="28"/>
       <c r="C15" s="8">
         <v>8.06</v>
       </c>
@@ -1518,30 +1610,30 @@
         <f t="shared" si="0"/>
         <v>8.06</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="I15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="11">
         <v>2392463</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="B16" s="28"/>
       <c r="C16" s="8">
         <v>2.61</v>
       </c>
@@ -1552,23 +1644,23 @@
         <f t="shared" si="0"/>
         <v>2.61</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="I16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16" s="11">
         <v>1663929</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1577,7 +1669,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="33"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -1586,9 +1678,9 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="B18" s="28"/>
       <c r="C18" s="8">
         <v>0.52</v>
       </c>
@@ -1596,31 +1688,31 @@
         <v>1</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" ref="E18:E23" si="1">C18*D18</f>
+        <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="I18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="11">
         <v>1607719</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8">
@@ -1630,33 +1722,33 @@
         <v>2</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.30199999999999999</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="I19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="K19" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="B20" s="28"/>
       <c r="C20" s="8">
         <v>4.74</v>
       </c>
@@ -1664,31 +1756,31 @@
         <v>2</v>
       </c>
       <c r="E20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.48</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="9" t="s">
+      <c r="K20" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8">
@@ -1698,33 +1790,33 @@
         <v>2</v>
       </c>
       <c r="E21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="I21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="K21" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="B22" s="28"/>
       <c r="C22" s="8">
         <v>5.91E-2</v>
       </c>
@@ -1732,33 +1824,33 @@
         <v>4</v>
       </c>
       <c r="E22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.2364</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>77</v>
+      <c r="F22" s="30" t="s">
+        <v>75</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" s="11">
         <v>1621821</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="B23" s="28"/>
       <c r="C23" s="8">
         <v>0.79700000000000004</v>
       </c>
@@ -1766,64 +1858,64 @@
         <v>4</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.1880000000000002</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="15" t="s">
+      <c r="K23" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="E24" s="10">
         <v>0</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="I24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8">
@@ -1833,26 +1925,26 @@
         <v>4</v>
       </c>
       <c r="E25" s="10">
-        <f>C25*D25</f>
+        <f t="shared" si="0"/>
         <v>1.1759999999999999</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1861,7 +1953,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="33"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="9"/>
       <c r="H26" s="15"/>
       <c r="I26" s="9"/>
@@ -1870,580 +1962,729 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="I27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="11" t="s">
+      <c r="K27" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="10">
+        <v>91</v>
+      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="8">
         <v>0.83</v>
       </c>
       <c r="D28" s="9">
         <v>2</v>
       </c>
       <c r="E28" s="10">
-        <f>C28*D28</f>
+        <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
-      <c r="F28" s="32" t="s">
+      <c r="F28" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="K28" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="27">
+      <c r="C29" s="25">
         <v>0.77500000000000002</v>
       </c>
       <c r="D29" s="11">
         <v>2</v>
       </c>
       <c r="E29" s="10">
-        <f t="shared" ref="E29:E34" si="2">C29*D29</f>
+        <f t="shared" si="0"/>
         <v>1.55</v>
       </c>
-      <c r="F29" s="33" t="s">
-        <v>151</v>
+      <c r="F29" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="G29" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H29" s="15" t="s">
-        <v>153</v>
-      </c>
       <c r="I29" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="1"/>
+      <c r="A30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="25">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="D30" s="38">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="0"/>
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>86</v>
+      <c r="A31" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="25">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="D31" s="40">
+        <v>1</v>
       </c>
       <c r="E31" s="10">
-        <v>0</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="11">
-        <v>2320821</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>160</v>
+        <f t="shared" si="0"/>
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="27">
-        <v>5.0299999999999997E-2</v>
-      </c>
-      <c r="D32" s="11">
-        <v>3</v>
+      <c r="A32" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="25">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D32" s="38">
+        <v>2</v>
       </c>
       <c r="E32" s="10">
-        <v>0</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="11">
-        <v>2320853</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>143</v>
+        <f t="shared" si="0"/>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="27">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="D33" s="11">
-        <v>3</v>
-      </c>
-      <c r="E33" s="10">
-        <f t="shared" si="2"/>
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="F33" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="11">
-        <v>2611941</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>148</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="31"/>
+        <v>93</v>
+      </c>
+      <c r="B34" s="7"/>
       <c r="C34" s="8">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="D34" s="11">
-        <v>3</v>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="2"/>
-        <v>1.44E-2</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>122</v>
+        <v>17</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" s="11">
-        <v>9334190</v>
+        <v>2320821</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="8">
-        <v>0.17399999999999999</v>
+        <v>94</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="25">
+        <v>5.0299999999999997E-2</v>
       </c>
       <c r="D35" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" s="10">
-        <f>C35*D35</f>
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="F35" s="33" t="s">
-        <v>124</v>
+        <f t="shared" si="0"/>
+        <v>0.15089999999999998</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>126</v>
+        <v>17</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J35" s="11">
-        <v>9550224</v>
+        <v>2320853</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="8">
-        <v>0.19900000000000001</v>
+        <v>116</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="25">
+        <v>0.13100000000000001</v>
       </c>
       <c r="D36" s="11">
         <v>3</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" ref="E36:E37" si="3">C36*D36</f>
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="F36" s="33" t="s">
-        <v>128</v>
+        <f t="shared" si="0"/>
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>142</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>129</v>
+        <v>70</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="J36" s="11">
+        <v>2611941</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="8">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D37" s="11">
+        <v>3</v>
+      </c>
+      <c r="E37" s="10">
+        <f t="shared" si="0"/>
+        <v>1.44E-2</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="11">
+        <v>9334190</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="8">
-        <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="D37" s="11">
-        <v>1</v>
-      </c>
-      <c r="E37" s="10">
-        <f t="shared" si="3"/>
-        <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="11">
-        <v>2303574</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="27" t="s">
+      <c r="B38" s="13"/>
+      <c r="C38" s="8">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="D38" s="11">
+        <v>4</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="0"/>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F38" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="11">
-        <v>1</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>121</v>
+      <c r="G38" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>121</v>
+        <v>19</v>
+      </c>
+      <c r="J38" s="11">
+        <v>9550224</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="31"/>
+        <v>111</v>
+      </c>
+      <c r="B39" s="13"/>
       <c r="C39" s="8">
-        <v>6.0000000000000001E-3</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="D39" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" s="10">
-        <f>C39*D39</f>
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>139</v>
+        <f t="shared" si="0"/>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>125</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J39" s="9">
-        <v>2447716</v>
+        <v>23</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="C40" s="8">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D40" s="11">
+        <v>1</v>
+      </c>
+      <c r="E40" s="10">
+        <f t="shared" si="0"/>
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="11">
+        <v>2303574</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="28"/>
+      <c r="C41" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="9">
+        <v>2447716</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="21">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="D44" s="22">
+        <v>1</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="0"/>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H44" s="49">
+        <v>694108301002</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="10">
-        <v>0</v>
-      </c>
-      <c r="F40" s="33" t="s">
+      <c r="K44" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="39"/>
+      <c r="C45" s="10">
+        <v>51.56</v>
+      </c>
+      <c r="D45" s="22">
+        <v>1</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="0"/>
+        <v>51.56</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="22">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="D41" s="23">
+      <c r="H45" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K45" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="47"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="43"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="39"/>
+      <c r="C47" s="10">
+        <v>1.41</v>
+      </c>
+      <c r="D47" s="22">
         <v>1</v>
       </c>
-      <c r="E41" s="10">
-        <f>C41*D41</f>
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="G41" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="H41" s="25">
-        <v>694108301002</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J41" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="K41" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="10">
-        <v>51.56</v>
-      </c>
-      <c r="D42" s="23">
-        <v>1</v>
-      </c>
-      <c r="E42" s="10">
-        <f>C42*D42</f>
-        <v>51.56</v>
-      </c>
-      <c r="F42" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H42" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="18"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E44" s="10">
-        <f>SUM(E8:E42)</f>
-        <v>84.427600000000012</v>
-      </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I45" s="17"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G46" s="21"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C47" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G47" s="1"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="1"/>
+      <c r="E47" s="10">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="11">
+        <v>3712278</v>
+      </c>
+      <c r="K47" s="22" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C48" s="9" t="s">
-        <v>112</v>
-      </c>
+      <c r="C48" s="18"/>
       <c r="I48" s="17"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="9" t="s">
-        <v>113</v>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="10">
+        <f>SUM(E8:E45)</f>
+        <v>85.216499999999996</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C50" s="30"/>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I50" s="17"/>
       <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G51" s="20"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="I53" s="17"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I54" s="17"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="27"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added all the remaining footprints to the schematic and exported the netlist.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -110,15 +110,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>1 nF Cap (0805)</t>
-  </si>
-  <si>
-    <t>MC0805B102K500CT</t>
-  </si>
-  <si>
-    <t>http://uk.farnell.com/multicomp/mc0805b102k500ct/cap-mlcc-x7r-1nf-50v-0805/dp/1759226</t>
-  </si>
-  <si>
     <t>C2, C3, C4</t>
   </si>
   <si>
@@ -659,6 +650,15 @@
   <si>
     <t>4 (Dup)</t>
   </si>
+  <si>
+    <t>1 nF Cap (0603)</t>
+  </si>
+  <si>
+    <t>MC0603B102K250CT</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/multicomp/mc0603b102k250ct/cap-mlcc-x7r-1000pf-25v-0603/dp/2627426</t>
+  </si>
 </sst>
 </file>
 
@@ -669,7 +669,7 @@
     <numFmt numFmtId="165" formatCode="\£#,##0.00;[Red]&quot;-£&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\£#,##0.000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.000;[Red]\-[$£-809]#,##0.000"/>
-    <numFmt numFmtId="178" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.000000000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -713,7 +713,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,12 +766,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -839,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -895,13 +889,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -913,7 +906,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1266,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -1311,10 +1304,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="6"/>
       <c r="J4" s="1"/>
     </row>
@@ -1373,7 +1366,7 @@
         <v>2.46E-2</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>17</v>
@@ -1413,7 +1406,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>19</v>
@@ -1422,7 +1415,7 @@
         <v>2447587</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1441,7 +1434,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>17</v>
@@ -1465,37 +1458,37 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="12">
-        <v>1.7600000000000001E-2</v>
+        <v>8.0999999999999996E-3</v>
       </c>
       <c r="D11" s="9">
         <v>1</v>
       </c>
       <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>1.7600000000000001E-2</v>
+        <v>8.0999999999999996E-3</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="11">
-        <v>1759226</v>
+        <v>2627426</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8">
@@ -1509,13 +1502,13 @@
         <v>0.11399999999999999</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>19</v>
@@ -1524,14 +1517,14 @@
         <v>2320821</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="13"/>
+        <v>140</v>
+      </c>
+      <c r="B13" s="28"/>
       <c r="C13" s="8">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -1543,27 +1536,27 @@
         <v>0.36</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="8">
@@ -1577,13 +1570,13 @@
         <v>0.75600000000000001</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>19</v>
@@ -1592,12 +1585,12 @@
         <v>8044953</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="8">
@@ -1611,13 +1604,13 @@
         <v>8.06</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>19</v>
@@ -1626,12 +1619,12 @@
         <v>2392463</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="8">
@@ -1645,13 +1638,13 @@
         <v>2.61</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>19</v>
@@ -1660,7 +1653,7 @@
         <v>1663929</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1678,7 +1671,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="8">
@@ -1692,13 +1685,13 @@
         <v>0.52</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>19</v>
@@ -1707,12 +1700,12 @@
         <v>1607719</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8">
@@ -1726,27 +1719,27 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="8">
@@ -1760,27 +1753,27 @@
         <v>9.48</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8">
@@ -1794,27 +1787,27 @@
         <v>0.16</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="8">
@@ -1828,13 +1821,13 @@
         <v>0.2364</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>19</v>
@@ -1843,12 +1836,12 @@
         <v>1621821</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="8">
@@ -1862,60 +1855,60 @@
         <v>3.1880000000000002</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="13"/>
+        <v>80</v>
+      </c>
+      <c r="B24" s="28"/>
       <c r="C24" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E24" s="10">
         <v>0</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8">
@@ -1929,22 +1922,22 @@
         <v>1.1759999999999999</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1962,42 +1955,42 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="B27" s="28"/>
       <c r="C27" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="35"/>
+        <v>88</v>
+      </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="8">
         <v>0.83</v>
       </c>
@@ -2009,29 +2002,29 @@
         <v>1.66</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="13"/>
+        <v>89</v>
+      </c>
+      <c r="B29" s="28"/>
       <c r="C29" s="25">
         <v>0.77500000000000002</v>
       </c>
@@ -2043,33 +2036,33 @@
         <v>1.55</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G29" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>147</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>150</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B30" s="13"/>
+        <v>158</v>
+      </c>
+      <c r="B30" s="28"/>
       <c r="C30" s="25">
         <v>0.36599999999999999</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="37">
         <v>1</v>
       </c>
       <c r="E30" s="10">
@@ -2077,33 +2070,33 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="39"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="25">
         <v>0.19800000000000001</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="39">
         <v>1</v>
       </c>
       <c r="E31" s="10">
@@ -2111,33 +2104,33 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="25">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D32" s="37">
         <v>2</v>
       </c>
       <c r="E32" s="10">
@@ -2145,22 +2138,22 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2178,26 +2171,26 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E34" s="10">
         <v>0</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>19</v>
@@ -2206,12 +2199,12 @@
         <v>2320821</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="25">
@@ -2225,13 +2218,13 @@
         <v>0.15089999999999998</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>19</v>
@@ -2240,12 +2233,12 @@
         <v>2320853</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="25">
@@ -2259,13 +2252,13 @@
         <v>0.39300000000000002</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>19</v>
@@ -2274,12 +2267,12 @@
         <v>2611941</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="8">
@@ -2293,13 +2286,13 @@
         <v>1.44E-2</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>19</v>
@@ -2308,14 +2301,14 @@
         <v>9334190</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="13"/>
+        <v>112</v>
+      </c>
+      <c r="B38" s="28"/>
       <c r="C38" s="8">
         <v>0.17399999999999999</v>
       </c>
@@ -2327,13 +2320,13 @@
         <v>0.69599999999999995</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>19</v>
@@ -2342,14 +2335,14 @@
         <v>9550224</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="13"/>
+        <v>108</v>
+      </c>
+      <c r="B39" s="28"/>
       <c r="C39" s="8">
         <v>0.19900000000000001</v>
       </c>
@@ -2361,27 +2354,27 @@
         <v>0.59699999999999998</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B40" s="28"/>
       <c r="C40" s="8">
@@ -2395,13 +2388,13 @@
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>19</v>
@@ -2410,16 +2403,16 @@
         <v>2303574</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B41" s="28"/>
       <c r="C41" s="25" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D41" s="11">
         <v>1</v>
@@ -2428,27 +2421,27 @@
         <v>0</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B42" s="28"/>
       <c r="C42" s="8">
@@ -2462,13 +2455,13 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>19</v>
@@ -2477,47 +2470,47 @@
         <v>2447716</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="B43" s="28"/>
       <c r="C43" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E43" s="10">
         <v>0</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B44" s="13"/>
+        <v>155</v>
+      </c>
+      <c r="B44" s="28"/>
       <c r="C44" s="21">
         <v>0.89200000000000002</v>
       </c>
@@ -2529,29 +2522,29 @@
         <v>0.89200000000000002</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G44" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="H44" s="49">
+        <v>95</v>
+      </c>
+      <c r="H44" s="48">
         <v>694108301002</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J44" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K44" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="39"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="10">
         <v>51.56</v>
       </c>
@@ -2563,42 +2556,42 @@
         <v>51.56</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H45" s="23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K45" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="44"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="43"/>
       <c r="G46" s="27"/>
-      <c r="H46" s="45"/>
+      <c r="H46" s="44"/>
       <c r="I46" s="27"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="43"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="42"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="10">
         <v>1.41</v>
       </c>
@@ -2610,13 +2603,13 @@
         <v>1.41</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>19</v>
@@ -2625,7 +2618,7 @@
         <v>3712278</v>
       </c>
       <c r="K47" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2635,11 +2628,11 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E49" s="10">
         <f>SUM(E8:E45)</f>
-        <v>85.216499999999996</v>
+        <v>85.206999999999994</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="1"/>
@@ -2650,10 +2643,10 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G51" s="20"/>
       <c r="I51" s="17"/>
@@ -2661,7 +2654,7 @@
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C52" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G52" s="1"/>
       <c r="I52" s="17"/>
@@ -2669,14 +2662,14 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C53" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I53" s="17"/>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C54" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I54" s="17"/>
       <c r="J54" s="1"/>

</xml_diff>

<commit_message>
Final adjustments made to PCB layout. PCB printing files created. BOM updated now that components have arrived.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -661,10 +661,10 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="\£#,##0.000;[Red]&quot;-£&quot;#,##0.000"/>
     <numFmt numFmtId="165" formatCode="\£#,##0.00;[Red]&quot;-£&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="[$£-809]#,##0.000;[Red]\-[$£-809]#,##0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000000000E+00"/>
-    <numFmt numFmtId="169" formatCode="\£#,##0.0000;[Red]&quot;-£&quot;#,##0.0000"/>
-    <numFmt numFmtId="170" formatCode="\£#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="[$£-809]#,##0.000;[Red]\-[$£-809]#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.0000;[Red]&quot;-£&quot;#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="\£#,##0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -715,7 +715,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,12 +766,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
@@ -779,18 +773,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
@@ -835,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -863,7 +845,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -886,13 +868,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -904,14 +885,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,10 +1286,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="5"/>
       <c r="J4" s="1"/>
     </row>
@@ -1354,11 +1333,11 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="45">
+      <c r="C8" s="44">
         <v>1.23E-2</v>
       </c>
       <c r="D8" s="8">
@@ -1388,7 +1367,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="6"/>
@@ -1422,7 +1401,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="6"/>
@@ -1456,11 +1435,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="D11" s="8">
@@ -1490,7 +1469,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="6"/>
@@ -1524,7 +1503,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="24" t="s">
         <v>133</v>
       </c>
       <c r="B13" s="26"/>
@@ -1592,7 +1571,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="26"/>
@@ -1626,7 +1605,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="26"/>
@@ -1673,7 +1652,7 @@
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="26"/>
@@ -1707,7 +1686,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="24" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="6"/>
@@ -1741,7 +1720,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="24" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="26"/>
@@ -1775,7 +1754,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="6"/>
@@ -1809,7 +1788,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="24" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="26"/>
@@ -1843,7 +1822,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="24" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="26"/>
@@ -1877,7 +1856,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="24" t="s">
         <v>76</v>
       </c>
       <c r="B24" s="26"/>
@@ -1910,7 +1889,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="6"/>
@@ -1930,7 +1909,7 @@
       <c r="G25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="46" t="s">
         <v>175</v>
       </c>
       <c r="I25" s="8" t="s">
@@ -1957,7 +1936,7 @@
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="24" t="s">
         <v>80</v>
       </c>
       <c r="B27" s="26"/>
@@ -1990,7 +1969,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="6"/>
@@ -2024,7 +2003,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="24" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="26"/>
@@ -2065,7 +2044,7 @@
       <c r="C30" s="23">
         <v>0.36599999999999999</v>
       </c>
-      <c r="D30" s="33">
+      <c r="D30" s="32">
         <v>1</v>
       </c>
       <c r="E30" s="9">
@@ -2095,11 +2074,11 @@
       <c r="A31" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="23">
         <v>0.19800000000000001</v>
       </c>
-      <c r="D31" s="35">
+      <c r="D31" s="34">
         <v>1</v>
       </c>
       <c r="E31" s="9">
@@ -2129,11 +2108,11 @@
       <c r="A32" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="23">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D32" s="32">
         <v>2</v>
       </c>
       <c r="E32" s="9">
@@ -2173,7 +2152,7 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="6"/>
@@ -2206,7 +2185,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="26"/>
@@ -2240,7 +2219,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="24" t="s">
         <v>106</v>
       </c>
       <c r="B36" s="26"/>
@@ -2274,7 +2253,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="24" t="s">
         <v>85</v>
       </c>
       <c r="B37" s="26"/>
@@ -2308,7 +2287,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="24" t="s">
         <v>105</v>
       </c>
       <c r="B38" s="26"/>
@@ -2342,7 +2321,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="24" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="26"/>
@@ -2376,7 +2355,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="24" t="s">
         <v>102</v>
       </c>
       <c r="B40" s="26"/>
@@ -2443,7 +2422,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="24" t="s">
         <v>104</v>
       </c>
       <c r="B42" s="26"/>
@@ -2477,7 +2456,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="24" t="s">
         <v>86</v>
       </c>
       <c r="B43" s="26"/>
@@ -2510,7 +2489,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="24" t="s">
         <v>146</v>
       </c>
       <c r="B44" s="26"/>
@@ -2530,7 +2509,7 @@
       <c r="G44" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="43">
         <v>694108301002</v>
       </c>
       <c r="I44" s="8" t="s">
@@ -2544,10 +2523,10 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="34"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="9">
         <v>51.56</v>
       </c>
@@ -2578,23 +2557,23 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="39"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="38"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="40"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="25"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="38"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="37"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="9">
         <v>1.26</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM after first PCB had been made
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -715,7 +715,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +776,24 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -817,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -891,6 +909,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1354,7 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="47" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="6"/>
@@ -1367,7 +1388,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="47" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="6"/>
@@ -1401,7 +1422,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="47" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="6"/>
@@ -1435,7 +1456,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="6"/>
@@ -1469,7 +1490,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="47" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="6"/>
@@ -1503,7 +1524,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="47" t="s">
         <v>133</v>
       </c>
       <c r="B13" s="26"/>
@@ -1537,7 +1558,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="26"/>
@@ -1571,7 +1592,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="26"/>
@@ -1605,7 +1626,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="49" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="26"/>
@@ -1639,7 +1660,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="8"/>
@@ -1652,7 +1673,7 @@
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="26"/>
@@ -1686,7 +1707,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="47" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="6"/>
@@ -1720,7 +1741,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="49" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="26"/>
@@ -1754,7 +1775,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="6"/>
@@ -1788,7 +1809,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="47" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="26"/>
@@ -1822,7 +1843,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="49" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="26"/>
@@ -1856,7 +1877,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="47" t="s">
         <v>76</v>
       </c>
       <c r="B24" s="26"/>
@@ -1889,7 +1910,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="47" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="6"/>
@@ -1923,7 +1944,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
@@ -1936,7 +1957,7 @@
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="47" t="s">
         <v>80</v>
       </c>
       <c r="B27" s="26"/>
@@ -1969,7 +1990,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="48" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="6"/>
@@ -2003,7 +2024,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="48" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="26"/>
@@ -2037,7 +2058,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="32" t="s">
         <v>149</v>
       </c>
       <c r="B30" s="26"/>
@@ -2071,7 +2092,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="33"/>
@@ -2105,7 +2126,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="33"/>
@@ -2152,7 +2173,7 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="47" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="6"/>
@@ -2185,7 +2206,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="47" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="26"/>
@@ -2219,7 +2240,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="47" t="s">
         <v>106</v>
       </c>
       <c r="B36" s="26"/>
@@ -2253,7 +2274,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="47" t="s">
         <v>85</v>
       </c>
       <c r="B37" s="26"/>
@@ -2287,7 +2308,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="47" t="s">
         <v>105</v>
       </c>
       <c r="B38" s="26"/>

</xml_diff>

<commit_message>
Minor updates to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="186">
   <si>
     <t>Key</t>
   </si>
@@ -652,6 +652,18 @@
   </si>
   <si>
     <t>MCB0805R474KCT</t>
+  </si>
+  <si>
+    <t>Additionally:</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Speaker Cables</t>
+  </si>
+  <si>
+    <t>Decoupling Caps</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,6 +1307,15 @@
       <c r="E2" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="G2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1303,6 +1324,9 @@
       </c>
       <c r="E3" s="11" t="s">
         <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>184</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -2058,7 +2082,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="49" t="s">
         <v>149</v>
       </c>
       <c r="B30" s="26"/>
@@ -2092,7 +2116,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="33"/>

</xml_diff>

<commit_message>
Made some improvements to the PCB grounding
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="190">
   <si>
     <t>Key</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>C9, C10</t>
-  </si>
-  <si>
-    <t>C13, C16, C20</t>
   </si>
   <si>
     <t>C14, C17, C19</t>
@@ -615,9 +612,6 @@
     <t>2 (Dup)</t>
   </si>
   <si>
-    <t>3 (Dup)</t>
-  </si>
-  <si>
     <t>4 (Dup)</t>
   </si>
   <si>
@@ -664,6 +658,24 @@
   </si>
   <si>
     <t>Decoupling Caps</t>
+  </si>
+  <si>
+    <t>C13, C16, C20, C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>100 µF Cap (radial)</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/panasonic-electronic-components/eeufr1j101l/cap-alu-elec-100uf-63v-rad/dp/2079296</t>
+  </si>
+  <si>
+    <t>EEUFR1J101L</t>
+  </si>
+  <si>
+    <t>100kohm</t>
   </si>
 </sst>
 </file>
@@ -1272,15 +1284,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.85546875"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875"/>
     <col min="3" max="3" width="8.5703125"/>
     <col min="4" max="4" width="11.85546875"/>
     <col min="5" max="5" width="11.7109375"/>
@@ -1305,16 +1318,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" t="s">
         <v>183</v>
-      </c>
-      <c r="I2" t="s">
-        <v>185</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -1326,7 +1339,10 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="I3" t="s">
+        <v>189</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -1389,11 +1405,11 @@
         <v>2</v>
       </c>
       <c r="E8" s="9">
-        <f t="shared" ref="E8:E47" si="0">C8*D8</f>
+        <f t="shared" ref="E8:E48" si="0">C8*D8</f>
         <v>2.46E-2</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>17</v>
@@ -1433,7 +1449,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>19</v>
@@ -1442,7 +1458,7 @@
         <v>2447587</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1461,7 +1477,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>17</v>
@@ -1495,13 +1511,13 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>19</v>
@@ -1510,7 +1526,7 @@
         <v>2627426</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1535,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>19</v>
@@ -1544,12 +1560,12 @@
         <v>2320821</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="7">
@@ -1680,7 +1696,7 @@
         <v>1663929</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,7 +1768,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>19</v>
@@ -1761,7 +1777,7 @@
         <v>9406336</v>
       </c>
       <c r="K19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1909,7 +1925,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E24" s="9">
         <v>0</v>
@@ -1955,7 +1971,7 @@
         <v>17</v>
       </c>
       <c r="H25" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>19</v>
@@ -1964,7 +1980,7 @@
         <v>2447556</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1989,7 +2005,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E27" s="9">
         <v>0</v>
@@ -2029,22 +2045,22 @@
         <v>1.66</v>
       </c>
       <c r="F28" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="H28" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K28" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2063,27 +2079,27 @@
         <v>1.55</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="23">
@@ -2097,22 +2113,22 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="F30" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="G30" s="28" t="s">
-        <v>151</v>
-      </c>
       <c r="H30" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2131,22 +2147,22 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="F31" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2165,22 +2181,22 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2198,14 +2214,14 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E34" s="9">
         <v>0</v>
@@ -2217,7 +2233,7 @@
         <v>17</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>19</v>
@@ -2226,12 +2242,12 @@
         <v>2320821</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="23">
@@ -2245,13 +2261,13 @@
         <v>0.15089999999999998</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>19</v>
@@ -2260,12 +2276,12 @@
         <v>2320853</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="23">
@@ -2279,13 +2295,13 @@
         <v>0.53099999999999992</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>19</v>
@@ -2294,417 +2310,451 @@
         <v>1288204</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
-        <v>85</v>
+      <c r="A37" s="49" t="s">
+        <v>185</v>
       </c>
       <c r="B37" s="26"/>
-      <c r="C37" s="7">
-        <v>4.7999999999999996E-3</v>
+      <c r="C37" s="23">
+        <v>0.61699999999999999</v>
       </c>
       <c r="D37" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="9">
         <f t="shared" si="0"/>
-        <v>1.44E-2</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>123</v>
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>109</v>
+        <v>79</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J37" s="10">
-        <v>9334190</v>
+        <v>2079296</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>110</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="7">
-        <v>0.17399999999999999</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="D38" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" s="9">
         <f t="shared" si="0"/>
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>111</v>
+        <v>1.44E-2</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J38" s="10">
-        <v>9550224</v>
+        <v>9334190</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>101</v>
+      <c r="A39" s="47" t="s">
+        <v>104</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="7">
-        <v>0.19900000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="D39" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E39" s="9">
         <f t="shared" si="0"/>
-        <v>0.59699999999999998</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>117</v>
+        <v>19</v>
+      </c>
+      <c r="J39" s="10">
+        <v>9550224</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="7">
-        <v>4.2599999999999999E-2</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="D40" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="9">
         <f t="shared" si="0"/>
-        <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>124</v>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="10">
-        <v>2303574</v>
+        <v>23</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41" s="26"/>
-      <c r="C41" s="23" t="s">
-        <v>108</v>
+      <c r="C41" s="7">
+        <v>4.2599999999999999E-2</v>
       </c>
       <c r="D41" s="10">
         <v>1</v>
       </c>
       <c r="E41" s="9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.2599999999999999E-2</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="J41" s="10">
+        <v>2303574</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42" s="26"/>
-      <c r="C42" s="7">
-        <v>6.0000000000000001E-3</v>
+      <c r="C42" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="D42" s="10">
         <v>1</v>
       </c>
       <c r="E42" s="9">
-        <f t="shared" si="0"/>
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="8">
-        <v>2447716</v>
+        <v>106</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="7">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>168</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D43" s="10">
+        <v>1</v>
       </c>
       <c r="E43" s="9">
-        <v>0</v>
-      </c>
-      <c r="F43" s="28" t="s">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="J43" s="8">
+        <v>2447716</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="B44" s="26"/>
-      <c r="C44" s="19">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="D44" s="20">
-        <v>1</v>
+      <c r="C44" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="E44" s="9">
-        <f t="shared" si="0"/>
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="F44" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G44" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="H44" s="43">
-        <v>694108301002</v>
+        <v>0</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K44" s="20" t="s">
-        <v>90</v>
+      <c r="J44" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="9">
-        <v>51.56</v>
+      <c r="A45" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="19">
+        <v>0.89200000000000002</v>
       </c>
       <c r="D45" s="20">
         <v>1</v>
       </c>
       <c r="E45" s="9">
         <f t="shared" si="0"/>
-        <v>51.56</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>92</v>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" s="43">
+        <v>694108301002</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="K45" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="33"/>
+      <c r="C46" s="9">
+        <v>51.56</v>
+      </c>
+      <c r="D46" s="20">
+        <v>1</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" si="0"/>
+        <v>51.56</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K45" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="37"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="41"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="37"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="9">
+      <c r="B48" s="33"/>
+      <c r="C48" s="9">
         <v>1.26</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D48" s="20">
         <v>1</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E48" s="9">
         <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
-      <c r="F47" s="28" t="s">
+      <c r="F48" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G48" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="H48" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="I48" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="10">
+        <v>3712278</v>
+      </c>
+      <c r="K48" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I47" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="10">
-        <v>3712278</v>
-      </c>
-      <c r="K47" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C48" s="16"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="1"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="9">
-        <f>SUM(E8:E45)</f>
-        <v>84.336000000000013</v>
-      </c>
+      <c r="C49" s="16"/>
       <c r="I49" s="15"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="9">
+        <f>SUM(E8:E48)</f>
+        <v>86.213000000000008</v>
+      </c>
       <c r="I50" s="15"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G51" s="18"/>
       <c r="I51" s="15"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="C52" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G52" s="18"/>
       <c r="I52" s="15"/>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C53" s="8" t="s">
-        <v>99</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="G53" s="1"/>
       <c r="I53" s="15"/>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C54" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I54" s="15"/>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C55" s="25"/>
+      <c r="C55" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="I55" s="15"/>
       <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="25"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>